<commit_message>
updating doc datasets for june event
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220715_Readme_NPOC_TN_COMPASS_TEMPEST_JUNE22_n6.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220715_Readme_NPOC_TN_COMPASS_TEMPEST_JUNE22_n6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25524"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl.sharepoint.com/teams/MCRL-COMPASS/Shared Documents/COMPASS Data Files MCRL/Raw_Instrument_Data/TEMPEST/TOC_LC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/OneDrive - PNNL/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{4F0C4E36-18BF-0349-84FF-F621AAAAB339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E4873D-67E7-4767-9C0C-7ADF5442A046}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6110F7-5A53-8E47-A20C-CB62126D435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15720" activeTab="1" xr2:uid="{DEC488EC-AAE5-5844-B3A3-F79197600DCD}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15720" xr2:uid="{DEC488EC-AAE5-5844-B3A3-F79197600DCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,30 +98,12 @@
     <t>NPOC: 1.142 mg/L, TN: 1.052 mg/L</t>
   </si>
   <si>
-    <t>FW_SOURCE_HR4</t>
-  </si>
-  <si>
-    <t>ESTUARY_BARGE_HR8</t>
-  </si>
-  <si>
-    <t>FW_SOURCE_HR5</t>
-  </si>
-  <si>
     <t>Omit</t>
   </si>
   <si>
     <t>NO PEAK, ran on 20220629 (no N but C peaks good)</t>
   </si>
   <si>
-    <t>FW_SOURCE_HR7</t>
-  </si>
-  <si>
-    <t>SW_SOURCE_HR7</t>
-  </si>
-  <si>
-    <t>FW_SOURCE_HR0</t>
-  </si>
-  <si>
     <t>Blank2</t>
   </si>
   <si>
@@ -156,13 +138,31 @@
   </si>
   <si>
     <t>*two different glass thickness-&gt; explains differing vial wts</t>
+  </si>
+  <si>
+    <t>TMP_FW_SOURCE_HR4</t>
+  </si>
+  <si>
+    <t>TMP_ESTUARY_BARGE_HR8</t>
+  </si>
+  <si>
+    <t>TMP_FW_SOURCE_HR5</t>
+  </si>
+  <si>
+    <t>TMP_FW_SOURCE_HR7</t>
+  </si>
+  <si>
+    <t>TMP_SW_SOURCE_HR7</t>
+  </si>
+  <si>
+    <t>TMP_FW_SOURCE_HR0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -532,17 +532,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97D79BB-A0FA-2148-AD15-817B5F87A5C6}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -573,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -589,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -600,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -611,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -622,7 +622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -633,92 +633,92 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -730,38 +730,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA30DBD-A0A6-4CE3-B81E-1F422D0C8866}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -770,18 +770,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -955,13 +955,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C4F001B-E43C-43A3-9B3A-40EB1C9D032C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE7E638A-E9EB-484B-9A5A-286234E24E09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE7E638A-E9EB-484B-9A5A-286234E24E09}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C4F001B-E43C-43A3-9B3A-40EB1C9D032C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D29851-37DD-430D-80F2-1D469092F61E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D29851-37DD-430D-80F2-1D469092F61E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>